<commit_message>
Crossing SI and GRM
</commit_message>
<xml_diff>
--- a/data/WOP_2026_planning.xlsx
+++ b/data/WOP_2026_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2026_winter\2026_winter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06121EA-1A51-40FA-BEBC-4E7695A1EBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8EAAC9-5ED8-4D12-BCA9-82F5529E08C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="585" windowWidth="29805" windowHeight="18810" activeTab="5" xr2:uid="{D40C415E-5EC6-489A-8663-B1D283C6BF70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{D40C415E-5EC6-489A-8663-B1D283C6BF70}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">map!$A$1:$W$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
Created biomass sample randomization
</commit_message>
<xml_diff>
--- a/data/WOP_2026_planning.xlsx
+++ b/data/WOP_2026_planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2026_winter\2026_winter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8EAAC9-5ED8-4D12-BCA9-82F5529E08C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58999C61-2167-47B2-88A8-C8077B337CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{D40C415E-5EC6-489A-8663-B1D283C6BF70}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15285" activeTab="5" xr2:uid="{D40C415E-5EC6-489A-8663-B1D283C6BF70}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">map!$A$1:$W$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>